<commit_message>
Complete Nani's TIMSS 2015 data
</commit_message>
<xml_diff>
--- a/RA/Nani_2022/T_19/T19_G4_5_Coding_explanation.xlsx
+++ b/RA/Nani_2022/T_19/T19_G4_5_Coding_explanation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Dropbox (UiO)\Nani\2022\T_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACC4F1C-49CD-4272-88E5-90F6B352455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FB6DCB-3C10-4ADC-8129-05B2627539DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="730" activeTab="2" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="730" activeTab="1" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
   </bookViews>
   <sheets>
     <sheet name="1_G4_PV" sheetId="14" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3279" uniqueCount="1815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3279" uniqueCount="1813">
   <si>
     <t>IDCNTRY</t>
   </si>
@@ -5250,9 +5250,6 @@
     <t>Access to learning management system</t>
   </si>
   <si>
-    <t>(1=0) (2=1) (3=1) (4=3) (5=4)</t>
-  </si>
-  <si>
     <t>(1=3) (2=2) (3=1) (4=0)</t>
   </si>
   <si>
@@ -5425,9 +5422,6 @@
   </si>
   <si>
     <t>IDXseasC</t>
-  </si>
-  <si>
-    <t>(0=3) (1=2) (2=1) (3=0)</t>
   </si>
   <si>
     <t>TOTWGT</t>
@@ -5521,7 +5515,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5540,6 +5534,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5553,7 +5553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5592,6 +5592,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5921,7 +5930,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A2:XFD23"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7481,14 +7490,14 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B94" s="11"/>
       <c r="C94" s="12" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="E94" s="11"/>
       <c r="F94" s="13">
@@ -7500,14 +7509,14 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B95" s="11"/>
       <c r="C95" s="12" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="E95" s="11"/>
       <c r="F95" s="13">
@@ -7519,14 +7528,14 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="B96" s="11"/>
       <c r="C96" s="12" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="E96" s="11"/>
       <c r="F96" s="13">
@@ -7538,14 +7547,14 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B97" s="11"/>
       <c r="C97" s="12" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="E97" s="11"/>
       <c r="F97" s="13">
@@ -7557,14 +7566,14 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="12" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="E98" s="11"/>
       <c r="F98" s="13">
@@ -7789,9 +7798,9 @@
   </sheetPr>
   <dimension ref="A1:G158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7941,7 +7950,7 @@
         <v>886</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F8" s="2">
         <v>9</v>
@@ -8185,7 +8194,7 @@
         <v>338</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>1481</v>
@@ -8208,7 +8217,7 @@
         <v>339</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>1482</v>
@@ -8286,7 +8295,7 @@
         <v>898</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F23" s="2">
         <v>9</v>
@@ -8309,7 +8318,7 @@
         <v>899</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F24" s="2">
         <v>9</v>
@@ -8332,7 +8341,7 @@
         <v>900</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F25" s="2">
         <v>9</v>
@@ -8355,7 +8364,7 @@
         <v>901</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F26" s="2">
         <v>9</v>
@@ -8378,7 +8387,7 @@
         <v>902</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F27" s="2">
         <v>9</v>
@@ -8401,7 +8410,7 @@
         <v>903</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F28" s="2">
         <v>9</v>
@@ -8424,7 +8433,7 @@
         <v>904</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F29" s="2">
         <v>9</v>
@@ -8447,7 +8456,7 @@
         <v>905</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F30" s="2">
         <v>9</v>
@@ -8470,7 +8479,7 @@
         <v>906</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F31" s="2">
         <v>9</v>
@@ -8493,7 +8502,7 @@
         <v>907</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F32" s="2">
         <v>9</v>
@@ -8516,7 +8525,7 @@
         <v>908</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F33" s="2">
         <v>9</v>
@@ -8539,7 +8548,7 @@
         <v>909</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F34" s="2">
         <v>9</v>
@@ -8556,13 +8565,13 @@
         <v>1496</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>910</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F35" s="2">
         <v>9</v>
@@ -8585,7 +8594,7 @@
         <v>911</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F36" s="2">
         <v>9</v>
@@ -8602,13 +8611,13 @@
         <v>1496</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>912</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F37" s="2">
         <v>9</v>
@@ -8625,13 +8634,13 @@
         <v>1496</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>913</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F38" s="2">
         <v>9</v>
@@ -8654,7 +8663,7 @@
         <v>914</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F39" s="2">
         <v>9</v>
@@ -8677,7 +8686,7 @@
         <v>915</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F40" s="2">
         <v>9</v>
@@ -8700,7 +8709,7 @@
         <v>916</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F41" s="2">
         <v>9</v>
@@ -8723,7 +8732,7 @@
         <v>917</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F42" s="2">
         <v>9</v>
@@ -8746,7 +8755,7 @@
         <v>918</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F43" s="2">
         <v>9</v>
@@ -8769,7 +8778,7 @@
         <v>919</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F44" s="2">
         <v>9</v>
@@ -8792,7 +8801,7 @@
         <v>920</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F45" s="2">
         <v>9</v>
@@ -8815,7 +8824,7 @@
         <v>921</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F46" s="2">
         <v>9</v>
@@ -8838,7 +8847,7 @@
         <v>922</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F47" s="2">
         <v>9</v>
@@ -8861,7 +8870,7 @@
         <v>923</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F48" s="2">
         <v>9</v>
@@ -8884,7 +8893,7 @@
         <v>924</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F49" s="2">
         <v>9</v>
@@ -8907,7 +8916,7 @@
         <v>925</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F50" s="2">
         <v>9</v>
@@ -8916,141 +8925,141 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
         <v>370</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="14" t="s">
         <v>1550</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="15" t="s">
         <v>1515</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="14" t="s">
         <v>926</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F51" s="2">
-        <v>9</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="E51" s="14" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F51" s="16">
+        <v>9</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="14" t="s">
         <v>1550</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="15" t="s">
         <v>1516</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="14" t="s">
         <v>927</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F52" s="2">
-        <v>9</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="E52" s="14" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F52" s="16">
+        <v>9</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="14" t="s">
         <v>1550</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="15" t="s">
         <v>1517</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="14" t="s">
         <v>928</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F53" s="2">
-        <v>9</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="E53" s="14" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F53" s="16">
+        <v>9</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="14" t="s">
         <v>1550</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="15" t="s">
         <v>1518</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="14" t="s">
         <v>929</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F54" s="2">
-        <v>9</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="E54" s="14" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F54" s="16">
+        <v>9</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="14" t="s">
         <v>1550</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="15" t="s">
         <v>1519</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="14" t="s">
         <v>930</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F55" s="2">
-        <v>9</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="E55" s="14" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F55" s="16">
+        <v>9</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="14" t="s">
         <v>1550</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="15" t="s">
         <v>1520</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="14" t="s">
         <v>931</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F56" s="2">
-        <v>9</v>
-      </c>
-      <c r="G56" s="1" t="s">
+      <c r="E56" s="14" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F56" s="16">
+        <v>9</v>
+      </c>
+      <c r="G56" s="14" t="s">
         <v>1733</v>
       </c>
     </row>
@@ -9067,8 +9076,8 @@
       <c r="D57" s="1" t="s">
         <v>932</v>
       </c>
-      <c r="E57" s="11" t="s">
-        <v>1797</v>
+      <c r="E57" s="4" t="s">
+        <v>1738</v>
       </c>
       <c r="F57" s="2">
         <v>9</v>
@@ -9090,8 +9099,8 @@
       <c r="D58" s="1" t="s">
         <v>933</v>
       </c>
-      <c r="E58" s="11" t="s">
-        <v>1797</v>
+      <c r="E58" s="4" t="s">
+        <v>1738</v>
       </c>
       <c r="F58" s="2">
         <v>9</v>
@@ -9113,8 +9122,8 @@
       <c r="D59" s="1" t="s">
         <v>934</v>
       </c>
-      <c r="E59" s="11" t="s">
-        <v>1797</v>
+      <c r="E59" s="4" t="s">
+        <v>1738</v>
       </c>
       <c r="F59" s="2">
         <v>9</v>
@@ -9136,8 +9145,8 @@
       <c r="D60" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="E60" s="11" t="s">
-        <v>1797</v>
+      <c r="E60" s="4" t="s">
+        <v>1738</v>
       </c>
       <c r="F60" s="2">
         <v>9</v>
@@ -9159,8 +9168,8 @@
       <c r="D61" s="1" t="s">
         <v>936</v>
       </c>
-      <c r="E61" s="11" t="s">
-        <v>1797</v>
+      <c r="E61" s="4" t="s">
+        <v>1738</v>
       </c>
       <c r="F61" s="2">
         <v>9</v>
@@ -9182,8 +9191,8 @@
       <c r="D62" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="E62" s="11" t="s">
-        <v>1797</v>
+      <c r="E62" s="4" t="s">
+        <v>1738</v>
       </c>
       <c r="F62" s="2">
         <v>9</v>
@@ -9206,7 +9215,7 @@
         <v>938</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F63" s="2">
         <v>9</v>
@@ -9223,13 +9232,13 @@
         <v>1528</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>939</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F64" s="2">
         <v>9</v>
@@ -9252,7 +9261,7 @@
         <v>940</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F65" s="2">
         <v>9</v>
@@ -9275,7 +9284,7 @@
         <v>941</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F66" s="2">
         <v>9</v>
@@ -9298,7 +9307,7 @@
         <v>942</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F67" s="2">
         <v>9</v>
@@ -9321,7 +9330,7 @@
         <v>943</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F68" s="2">
         <v>9</v>
@@ -9344,7 +9353,7 @@
         <v>944</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F69" s="2">
         <v>9</v>
@@ -9361,13 +9370,13 @@
         <v>1528</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>945</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F70" s="2">
         <v>9</v>
@@ -9390,7 +9399,7 @@
         <v>946</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F71" s="2">
         <v>9</v>
@@ -9413,7 +9422,7 @@
         <v>947</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F72" s="2">
         <v>9</v>
@@ -9436,7 +9445,7 @@
         <v>948</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F73" s="2">
         <v>9</v>
@@ -9459,7 +9468,7 @@
         <v>949</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F74" s="2">
         <v>9</v>
@@ -9482,7 +9491,7 @@
         <v>950</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F75" s="2">
         <v>9</v>
@@ -9505,7 +9514,7 @@
         <v>951</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F76" s="2">
         <v>9</v>
@@ -9528,7 +9537,7 @@
         <v>952</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F77" s="2">
         <v>9</v>
@@ -9551,7 +9560,7 @@
         <v>953</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F78" s="2">
         <v>9</v>
@@ -9574,7 +9583,7 @@
         <v>954</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F79" s="2">
         <v>9</v>
@@ -9597,7 +9606,7 @@
         <v>955</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F80" s="2">
         <v>9</v>
@@ -9620,7 +9629,7 @@
         <v>956</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F81" s="2">
         <v>9</v>
@@ -9643,7 +9652,7 @@
         <v>957</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F82" s="2">
         <v>9</v>
@@ -9666,7 +9675,7 @@
         <v>958</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F83" s="2">
         <v>9</v>
@@ -9689,7 +9698,7 @@
         <v>959</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F84" s="2">
         <v>9</v>
@@ -9712,7 +9721,7 @@
         <v>960</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F85" s="2">
         <v>9</v>
@@ -9735,7 +9744,7 @@
         <v>961</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F86" s="2">
         <v>9</v>
@@ -9758,7 +9767,7 @@
         <v>962</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F87" s="2">
         <v>9</v>
@@ -9781,7 +9790,7 @@
         <v>963</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F88" s="2">
         <v>9</v>
@@ -9804,7 +9813,7 @@
         <v>964</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F89" s="2">
         <v>9</v>
@@ -9827,7 +9836,7 @@
         <v>965</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F90" s="2">
         <v>9</v>
@@ -9850,7 +9859,7 @@
         <v>966</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F91" s="2">
         <v>9</v>
@@ -9873,7 +9882,7 @@
         <v>967</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F92" s="2">
         <v>9</v>
@@ -9896,7 +9905,7 @@
         <v>968</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F93" s="2">
         <v>9</v>
@@ -9919,7 +9928,7 @@
         <v>969</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F94" s="2">
         <v>9</v>
@@ -9942,7 +9951,7 @@
         <v>970</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F95" s="2">
         <v>9</v>
@@ -10103,7 +10112,7 @@
         <v>977</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F102" s="2">
         <v>9</v>
@@ -10126,7 +10135,7 @@
         <v>978</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F103" s="2">
         <v>9</v>
@@ -10149,7 +10158,7 @@
         <v>979</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F104" s="2">
         <v>9</v>
@@ -10172,7 +10181,7 @@
         <v>980</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F105" s="2">
         <v>9</v>
@@ -10195,7 +10204,7 @@
         <v>981</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F106" s="2">
         <v>9</v>
@@ -10218,7 +10227,7 @@
         <v>982</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F107" s="2">
         <v>9</v>
@@ -10241,7 +10250,7 @@
         <v>983</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F108" s="2">
         <v>9</v>
@@ -10264,7 +10273,7 @@
         <v>984</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F109" s="2">
         <v>9</v>
@@ -10287,7 +10296,7 @@
         <v>985</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F110" s="2">
         <v>9</v>
@@ -10310,7 +10319,7 @@
         <v>986</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F111" s="2">
         <v>9</v>
@@ -10333,7 +10342,7 @@
         <v>987</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F112" s="2">
         <v>9</v>
@@ -10460,7 +10469,7 @@
         <v>1466</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>992</v>
@@ -10509,7 +10518,7 @@
         <v>994</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="F122" s="2">
         <v>9</v>
@@ -10520,10 +10529,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>1798</v>
+        <v>1796</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1801</v>
+        <v>1799</v>
       </c>
       <c r="F123" s="2">
         <v>999999</v>
@@ -10534,10 +10543,10 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="F124" s="2">
         <v>999999</v>
@@ -10548,10 +10557,10 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>1800</v>
+        <v>1798</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
       <c r="F125" s="2">
         <v>999999</v>
@@ -10708,7 +10717,7 @@
         <v>1002</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="F135" s="2">
         <v>9</v>
@@ -10811,7 +10820,7 @@
         <v>1703</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>1007</v>
@@ -10837,7 +10846,7 @@
         <v>1008</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="F141" s="2">
         <v>9</v>
@@ -11112,7 +11121,7 @@
         <v>1709</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D154" s="4" t="s">
         <v>1021</v>
@@ -11132,7 +11141,7 @@
         <v>1709</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>1022</v>
@@ -11227,9 +11236,9 @@
   </sheetPr>
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E222" sqref="E222"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A228" sqref="A228:XFD228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11924,13 +11933,13 @@
         <v>1134</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>675</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F38" s="2">
         <v>9</v>
@@ -11947,13 +11956,13 @@
         <v>1134</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>676</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F39" s="2">
         <v>9</v>
@@ -11970,13 +11979,13 @@
         <v>1134</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>677</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F40" s="2">
         <v>9</v>
@@ -11993,13 +12002,13 @@
         <v>1134</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>678</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F41" s="2">
         <v>9</v>
@@ -12016,13 +12025,13 @@
         <v>1134</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>679</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F42" s="2">
         <v>9</v>
@@ -12039,13 +12048,13 @@
         <v>1134</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>680</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F43" s="2">
         <v>9</v>
@@ -12062,13 +12071,13 @@
         <v>1134</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>681</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F44" s="2">
         <v>9</v>
@@ -12085,13 +12094,13 @@
         <v>1134</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>682</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F45" s="2">
         <v>9</v>
@@ -12108,13 +12117,13 @@
         <v>1134</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>683</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F46" s="2">
         <v>9</v>
@@ -12131,13 +12140,13 @@
         <v>1134</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>684</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F47" s="2">
         <v>9</v>
@@ -12154,13 +12163,13 @@
         <v>1134</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>685</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F48" s="2">
         <v>9</v>
@@ -12177,13 +12186,13 @@
         <v>1134</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>686</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="F49" s="2">
         <v>9</v>
@@ -12206,7 +12215,7 @@
         <v>687</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F50" s="2">
         <v>9</v>
@@ -12229,7 +12238,7 @@
         <v>688</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F51" s="2">
         <v>9</v>
@@ -12252,7 +12261,7 @@
         <v>689</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F52" s="2">
         <v>9</v>
@@ -12275,7 +12284,7 @@
         <v>690</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F53" s="2">
         <v>9</v>
@@ -12298,7 +12307,7 @@
         <v>691</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F54" s="2">
         <v>9</v>
@@ -12321,7 +12330,7 @@
         <v>692</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F55" s="2">
         <v>9</v>
@@ -12344,7 +12353,7 @@
         <v>693</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F56" s="2">
         <v>9</v>
@@ -12367,7 +12376,7 @@
         <v>694</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F57" s="2">
         <v>9</v>
@@ -12390,7 +12399,7 @@
         <v>695</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F58" s="2">
         <v>9</v>
@@ -12413,7 +12422,7 @@
         <v>696</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F59" s="2">
         <v>9</v>
@@ -12436,7 +12445,7 @@
         <v>697</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F60" s="2">
         <v>9</v>
@@ -12459,7 +12468,7 @@
         <v>698</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F61" s="2">
         <v>9</v>
@@ -12482,7 +12491,7 @@
         <v>699</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F62" s="2">
         <v>9</v>
@@ -12505,7 +12514,7 @@
         <v>700</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F63" s="2">
         <v>9</v>
@@ -12528,7 +12537,7 @@
         <v>701</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F64" s="2">
         <v>9</v>
@@ -12551,7 +12560,7 @@
         <v>702</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F65" s="2">
         <v>9</v>
@@ -12574,7 +12583,7 @@
         <v>703</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F66" s="2">
         <v>9</v>
@@ -12597,7 +12606,7 @@
         <v>704</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F67" s="2">
         <v>9</v>
@@ -12620,7 +12629,7 @@
         <v>705</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F68" s="2">
         <v>9</v>
@@ -12643,7 +12652,7 @@
         <v>706</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F69" s="2">
         <v>9</v>
@@ -12666,7 +12675,7 @@
         <v>707</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F70" s="2">
         <v>9</v>
@@ -12749,7 +12758,7 @@
         <v>711</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F74" s="2">
         <v>9</v>
@@ -12772,7 +12781,7 @@
         <v>712</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F75" s="2">
         <v>9</v>
@@ -12795,7 +12804,7 @@
         <v>713</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F76" s="2">
         <v>9</v>
@@ -12818,7 +12827,7 @@
         <v>714</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F77" s="2">
         <v>9</v>
@@ -12841,7 +12850,7 @@
         <v>715</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F78" s="2">
         <v>9</v>
@@ -12864,7 +12873,7 @@
         <v>716</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F79" s="2">
         <v>9</v>
@@ -12887,7 +12896,7 @@
         <v>717</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F80" s="2">
         <v>9</v>
@@ -12910,7 +12919,7 @@
         <v>718</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F81" s="2">
         <v>9</v>
@@ -13137,7 +13146,7 @@
         <v>728</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F91" s="2">
         <v>9</v>
@@ -13160,7 +13169,7 @@
         <v>729</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F92" s="2">
         <v>9</v>
@@ -13183,7 +13192,7 @@
         <v>730</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F93" s="2">
         <v>9</v>
@@ -13206,7 +13215,7 @@
         <v>731</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F94" s="2">
         <v>9</v>
@@ -13229,7 +13238,7 @@
         <v>732</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F95" s="2">
         <v>9</v>
@@ -13252,7 +13261,7 @@
         <v>733</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F96" s="2">
         <v>9</v>
@@ -13275,7 +13284,7 @@
         <v>734</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F97" s="2">
         <v>9</v>
@@ -13298,7 +13307,7 @@
         <v>735</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F98" s="2">
         <v>9</v>
@@ -13436,7 +13445,7 @@
         <v>741</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>1448</v>
@@ -13459,7 +13468,7 @@
         <v>742</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>1448</v>
@@ -13482,7 +13491,7 @@
         <v>743</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>1448</v>
@@ -13505,7 +13514,7 @@
         <v>744</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>1448</v>
@@ -14560,7 +14569,7 @@
         <v>790</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F153" s="2">
         <v>9</v>
@@ -14583,7 +14592,7 @@
         <v>791</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F154" s="2">
         <v>9</v>
@@ -14606,7 +14615,7 @@
         <v>792</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F155" s="2">
         <v>9</v>
@@ -14629,7 +14638,7 @@
         <v>793</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F156" s="2">
         <v>9</v>
@@ -14652,7 +14661,7 @@
         <v>794</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F157" s="2">
         <v>9</v>
@@ -14675,7 +14684,7 @@
         <v>795</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F158" s="2">
         <v>9</v>
@@ -14698,7 +14707,7 @@
         <v>796</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F159" s="2">
         <v>9</v>
@@ -14721,7 +14730,7 @@
         <v>797</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F160" s="2">
         <v>9</v>
@@ -14744,7 +14753,7 @@
         <v>798</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F161" s="2">
         <v>9</v>
@@ -14767,7 +14776,7 @@
         <v>799</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F162" s="2">
         <v>9</v>
@@ -14790,7 +14799,7 @@
         <v>800</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F163" s="2">
         <v>9</v>
@@ -14813,7 +14822,7 @@
         <v>801</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F164" s="2">
         <v>9</v>
@@ -14836,7 +14845,7 @@
         <v>802</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F165" s="2">
         <v>9</v>
@@ -14951,7 +14960,7 @@
         <v>807</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>1448</v>
@@ -14974,7 +14983,7 @@
         <v>808</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>1448</v>
@@ -14997,7 +15006,7 @@
         <v>809</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F172" s="2" t="s">
         <v>1448</v>
@@ -15020,7 +15029,7 @@
         <v>810</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>1448</v>
@@ -16072,7 +16081,7 @@
         <v>1438</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>1813</v>
+        <v>1811</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>856</v>
@@ -16095,7 +16104,7 @@
         <v>1438</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>857</v>
@@ -16262,7 +16271,7 @@
         <v>864</v>
       </c>
       <c r="E227" s="11" t="s">
-        <v>1738</v>
+        <v>1322</v>
       </c>
       <c r="F227" s="2">
         <v>9</v>
@@ -16313,7 +16322,7 @@
         <v>1439</v>
       </c>
       <c r="C230" s="12" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>867</v>
@@ -16333,7 +16342,7 @@
         <v>1439</v>
       </c>
       <c r="C231" s="12" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>868</v>
@@ -16701,8 +16710,8 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16853,7 +16862,7 @@
         <v>1029</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="F7" s="2">
         <v>99</v>
@@ -16936,7 +16945,7 @@
         <v>1033</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="F11" s="2">
         <v>9</v>
@@ -17545,7 +17554,7 @@
         <v>1663</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>1060</v>
@@ -17568,7 +17577,7 @@
         <v>1663</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>1061</v>
@@ -17591,7 +17600,7 @@
         <v>1663</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>1062</v>
@@ -17614,7 +17623,7 @@
         <v>1663</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>1063</v>
@@ -17637,7 +17646,7 @@
         <v>1663</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>1064</v>
@@ -17660,7 +17669,7 @@
         <v>1663</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>1065</v>
@@ -17683,7 +17692,7 @@
         <v>1663</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>1066</v>
@@ -17706,7 +17715,7 @@
         <v>1663</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>1067</v>
@@ -17729,7 +17738,7 @@
         <v>1663</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>1068</v>
@@ -17752,7 +17761,7 @@
         <v>1663</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>1069</v>
@@ -17775,7 +17784,7 @@
         <v>1663</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>1070</v>
@@ -18561,10 +18570,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>1804</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>1806</v>
       </c>
       <c r="F84" s="1">
         <v>999999</v>
@@ -18575,10 +18584,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>1805</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>1807</v>
       </c>
       <c r="F85" s="1">
         <v>999999</v>
@@ -18617,10 +18626,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>1808</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>1810</v>
       </c>
       <c r="F88" s="2">
         <v>9</v>
@@ -18631,10 +18640,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>1809</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>1811</v>
       </c>
       <c r="F89" s="2">
         <v>99</v>
@@ -18737,7 +18746,7 @@
         <v>1720</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>1107</v>
@@ -18757,7 +18766,7 @@
         <v>1720</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>1108</v>
@@ -18820,7 +18829,7 @@
         <v>555</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>1716</v>
@@ -18840,7 +18849,7 @@
         <v>556</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>1717</v>

</xml_diff>